<commit_message>
do not convert new line test
</commit_message>
<xml_diff>
--- a/example/app/i18n/languages.xlsx
+++ b/example/app/i18n/languages.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="127">
   <si>
     <t>string id</t>
   </si>
@@ -255,6 +255,24 @@
       </rPr>
       <t>[1]</t>
     </r>
+  </si>
+  <si>
+    <t>string_includes_new_line</t>
+  </si>
+  <si>
+    <t>new line</t>
+  </si>
+  <si>
+    <t>first line
+second line
+third line</t>
+  </si>
+  <si>
+    <t>string_includes_hard_coded_new_line</t>
+  </si>
+  <si>
+    <t>first hard coded line\nsecond hard coded line\nthird hard coded line
+last line with sheet new line</t>
   </si>
   <si>
     <t>[]string_array_03</t>
@@ -818,7 +836,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -847,6 +865,12 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1381,287 +1405,298 @@
       <c r="F18" s="7"/>
     </row>
     <row r="19" ht="12.75" customHeight="1">
-      <c r="A19" s="4"/>
-      <c r="B19" s="5"/>
-      <c r="D19" s="5"/>
+      <c r="A19" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>62</v>
+      </c>
       <c r="E19" s="5"/>
       <c r="F19" s="7"/>
     </row>
     <row r="20" ht="12.75" customHeight="1">
-      <c r="A20" s="4"/>
-      <c r="B20" s="5"/>
-      <c r="D20" s="5"/>
+      <c r="A20" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>64</v>
+      </c>
       <c r="E20" s="5"/>
       <c r="F20" s="7"/>
     </row>
     <row r="21" ht="12.75" customHeight="1">
-      <c r="A21" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>61</v>
-      </c>
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
+      <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="7"/>
     </row>
     <row r="22" ht="12.75" customHeight="1">
       <c r="A22" s="4" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>58</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="7"/>
     </row>
     <row r="23" ht="12.75" customHeight="1">
       <c r="A23" s="4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>58</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="7"/>
     </row>
     <row r="24" ht="12.75" customHeight="1">
       <c r="A24" s="4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>69</v>
+        <v>58</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>70</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="7"/>
     </row>
     <row r="25" ht="12.75" customHeight="1">
       <c r="A25" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="7"/>
     </row>
     <row r="26" ht="12.75" customHeight="1">
       <c r="A26" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="7"/>
     </row>
     <row r="27" ht="12.75" customHeight="1">
       <c r="A27" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="7"/>
     </row>
     <row r="28" ht="12.75" customHeight="1">
       <c r="A28" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="7"/>
     </row>
     <row r="29" ht="12.75" customHeight="1">
       <c r="A29" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="7"/>
     </row>
     <row r="30" ht="12.75" customHeight="1">
       <c r="A30" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="7"/>
     </row>
     <row r="31" ht="12.75" customHeight="1">
       <c r="A31" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="7"/>
     </row>
     <row r="32" ht="12.75" customHeight="1">
       <c r="A32" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="7"/>
     </row>
     <row r="33" ht="12.75" customHeight="1">
       <c r="A33" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="7"/>
     </row>
     <row r="34" ht="12.75" customHeight="1">
       <c r="A34" s="4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="7"/>
     </row>
     <row r="35" ht="12.75" customHeight="1">
       <c r="A35" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="7"/>
     </row>
     <row r="36" ht="12.75" customHeight="1">
       <c r="A36" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="7"/>
     </row>
     <row r="37" ht="12.75" customHeight="1">
       <c r="A37" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
+      <c r="F37" s="7"/>
     </row>
     <row r="38" ht="12.75" customHeight="1">
-      <c r="A38" s="4"/>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
+      <c r="A38" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>126</v>
+      </c>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
     </row>
@@ -1674,7 +1709,12 @@
       <c r="F39" s="5"/>
     </row>
     <row r="40" ht="12.75" customHeight="1">
-      <c r="A40" s="3"/>
+      <c r="A40" s="4"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
     </row>
     <row r="41" ht="12.75" customHeight="1">
       <c r="A41" s="3"/>
@@ -4555,6 +4595,9 @@
     </row>
     <row r="1000" ht="12.75" customHeight="1">
       <c r="A1000" s="3"/>
+    </row>
+    <row r="1001" ht="12.75" customHeight="1">
+      <c r="A1001" s="3"/>
     </row>
   </sheetData>
   <printOptions/>

</xml_diff>